<commit_message>
feat: leader board topic-xp-stats
</commit_message>
<xml_diff>
--- a/data/import/Exercise.xlsx
+++ b/data/import/Exercise.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\svNam4\HK2\4KidStudy\4kidstudy-backend\data\import\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B488CD4-7AEC-4DC3-8627-D3F7443285E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44D8A582-125B-490A-83DF-D084A3F0878C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{63998D71-9BE4-4E89-BA80-C31794CAC3F5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="36">
   <si>
     <t>type</t>
   </si>
@@ -66,9 +66,6 @@
   </si>
   <si>
     <t>SELECT_IMAGE</t>
-  </si>
-  <si>
-    <t>\n</t>
   </si>
   <si>
     <t>MULTIPLE_CHOICE</t>
@@ -532,7 +529,7 @@
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -587,174 +584,111 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" t="s">
         <v>23</v>
       </c>
-      <c r="C2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>24</v>
       </c>
-      <c r="I2" t="s">
-        <v>25</v>
-      </c>
       <c r="J2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" t="s">
         <v>11</v>
       </c>
-      <c r="B3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G3" t="s">
-        <v>28</v>
-      </c>
-      <c r="H3" t="s">
-        <v>29</v>
-      </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>12</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>13</v>
-      </c>
-      <c r="K3" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
         <v>15</v>
       </c>
-      <c r="B4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" t="s">
-        <v>10</v>
-      </c>
       <c r="D4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I4" t="s">
         <v>30</v>
       </c>
-      <c r="E4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" t="s">
-        <v>27</v>
-      </c>
-      <c r="G4" t="s">
-        <v>28</v>
-      </c>
-      <c r="H4" t="s">
-        <v>27</v>
-      </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>31</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>32</v>
-      </c>
-      <c r="K4" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
         <v>17</v>
       </c>
-      <c r="B5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" t="s">
-        <v>10</v>
-      </c>
       <c r="D5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E5" t="s">
-        <v>27</v>
-      </c>
-      <c r="F5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" t="s">
-        <v>10</v>
-      </c>
-      <c r="H5" t="s">
-        <v>10</v>
-      </c>
-      <c r="I5" t="s">
-        <v>10</v>
-      </c>
-      <c r="J5" t="s">
-        <v>10</v>
-      </c>
-      <c r="K5" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" t="s">
         <v>19</v>
       </c>
-      <c r="B6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6" t="s">
-        <v>10</v>
-      </c>
       <c r="H6" t="s">
+        <v>33</v>
+      </c>
+      <c r="I6" t="s">
         <v>34</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K6" t="s">
         <v>35</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="K6" t="s">
-        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>